<commit_message>
TS 3.2 Ghanam Tamil
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 3.4 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 3.4 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7A1BDC-C0C6-47E5-9461-1748E3580B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BCFEBC-2379-4F13-8CDB-75A8AD56FFF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5563,10 +5563,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2393"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A908" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="U2334" sqref="U2334"/>
+      <selection pane="bottomLeft" activeCell="N919" sqref="N919"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
TS 3.4 Ghanam and Jatai first review Raja output- 09/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 3.4 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 3.4 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A4EF31-1B04-42E0-AAF6-B3C8132C441D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482F7CA0-10E5-400B-8EB3-685BA1E97412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8585" uniqueCount="1618">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8563" uniqueCount="1619">
   <si>
     <t>PS</t>
   </si>
@@ -4890,19 +4890,28 @@
   </si>
   <si>
     <t>P%S[Sh]</t>
+  </si>
+  <si>
+    <t>ruqdriyaqm iti# ruqdriya$m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -5112,190 +5121,191 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5579,9 +5589,9 @@
   <dimension ref="A1:V2393"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2161" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="V2189" sqref="V2189"/>
+      <selection pane="bottomLeft" activeCell="V2175" sqref="V2175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -78476,8 +78486,8 @@
       <c r="P2175" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="V2175" s="36" t="s">
-        <v>1510</v>
+      <c r="V2175" s="63" t="s">
+        <v>1618</v>
       </c>
     </row>
     <row r="2176" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
nmv 15 10 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 3.4 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 3.4 Padam Input Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482F7CA0-10E5-400B-8EB3-685BA1E97412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D63D2F66-2F60-4297-8E83-7101AC49E6E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TS 3.4" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8563" uniqueCount="1619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8563" uniqueCount="1618">
   <si>
     <t>PS</t>
   </si>
@@ -4887,9 +4887,6 @@
   </si>
   <si>
     <t>sAqnaqsimiti# sAnaqsim</t>
-  </si>
-  <si>
-    <t>P%S[Sh]</t>
   </si>
   <si>
     <t>ruqdriyaqm iti# ruqdriya$m</t>
@@ -5121,7 +5118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -5299,13 +5296,16 @@
     <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5589,9 +5589,9 @@
   <dimension ref="A1:V2393"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2161" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1807" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="V2175" sqref="V2175"/>
+      <selection pane="bottomLeft" activeCell="S1821" sqref="S1821:T1821"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -68402,11 +68402,11 @@
       <c r="O1821" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="S1821" s="61" t="s">
+      <c r="S1821" s="63" t="s">
         <v>150</v>
       </c>
-      <c r="T1821" s="61" t="s">
-        <v>1617</v>
+      <c r="T1821" s="64" t="s">
+        <v>151</v>
       </c>
       <c r="V1821" s="36" t="s">
         <v>1615</v>
@@ -78486,8 +78486,8 @@
       <c r="P2175" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="V2175" s="63" t="s">
-        <v>1618</v>
+      <c r="V2175" s="62" t="s">
+        <v>1617</v>
       </c>
     </row>
     <row r="2176" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -78921,7 +78921,7 @@
       <c r="P2189" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="V2189" s="62" t="s">
+      <c r="V2189" s="61" t="s">
         <v>1585</v>
       </c>
     </row>

</xml_diff>

<commit_message>
nmv 18 10 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 3.4 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 3.4 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3040B813-1D19-444D-824F-1D9503FB6C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB2AE3C-7390-42A7-A935-6CE906C11E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8570" uniqueCount="1618">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8564" uniqueCount="1619">
   <si>
     <t>PS</t>
   </si>
@@ -4910,6 +4910,9 @@
       </rPr>
       <t>po$</t>
     </r>
+  </si>
+  <si>
+    <t>dyAqvAqpRuqthiqvyA$m</t>
   </si>
 </sst>
 </file>
@@ -5617,10 +5620,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2393"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A221" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A431" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="V233" sqref="V233"/>
+      <selection pane="bottomLeft" activeCell="Q446" sqref="Q446"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -22576,8 +22579,8 @@
         <f t="shared" si="20"/>
         <v>109</v>
       </c>
-      <c r="N444" s="36" t="s">
-        <v>226</v>
+      <c r="N444" s="61" t="s">
+        <v>1618</v>
       </c>
       <c r="O444" s="7" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
nmv 23 10 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 3.4 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 3.4 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2557445-3659-4997-BA08-0A2D5E3BBBA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC63860-C41E-43AC-B531-29F6EFE47EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8563" uniqueCount="1619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8562" uniqueCount="1619">
   <si>
     <t>PS</t>
   </si>
@@ -5356,9 +5356,6 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -5376,6 +5373,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5661,9 +5661,9 @@
   <dimension ref="A1:V2393"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1332" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1857" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N1336" sqref="N1336"/>
+      <selection pane="bottomLeft" activeCell="U1872" sqref="U1872"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -14997,7 +14997,7 @@
       <c r="S233" s="7"/>
       <c r="T233" s="7"/>
       <c r="U233" s="7"/>
-      <c r="V233" s="61" t="s">
+      <c r="V233" s="60" t="s">
         <v>1615</v>
       </c>
     </row>
@@ -15073,7 +15073,7 @@
       <c r="R235" s="7"/>
       <c r="S235" s="7"/>
       <c r="T235" s="7"/>
-      <c r="U235" s="65" t="s">
+      <c r="U235" s="64" t="s">
         <v>130</v>
       </c>
       <c r="V235" s="36" t="s">
@@ -22619,7 +22619,7 @@
         <f t="shared" si="20"/>
         <v>109</v>
       </c>
-      <c r="N444" s="61" t="s">
+      <c r="N444" s="60" t="s">
         <v>1616</v>
       </c>
       <c r="O444" s="7" t="s">
@@ -46524,7 +46524,7 @@
       <c r="S1133" s="7"/>
       <c r="T1133" s="7"/>
       <c r="U1133" s="7"/>
-      <c r="V1133" s="61" t="s">
+      <c r="V1133" s="60" t="s">
         <v>1617</v>
       </c>
     </row>
@@ -53401,7 +53401,7 @@
         <f t="shared" si="61"/>
         <v>203</v>
       </c>
-      <c r="N1336" s="61" t="s">
+      <c r="N1336" s="60" t="s">
         <v>1618</v>
       </c>
       <c r="O1336" s="7" t="s">
@@ -68473,10 +68473,10 @@
       <c r="O1821" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="S1821" s="63" t="s">
+      <c r="S1821" s="62" t="s">
         <v>150</v>
       </c>
-      <c r="T1821" s="64" t="s">
+      <c r="T1821" s="63" t="s">
         <v>151</v>
       </c>
       <c r="V1821" s="36" t="s">
@@ -69950,9 +69950,7 @@
       <c r="N1872" s="36" t="s">
         <v>954</v>
       </c>
-      <c r="U1872" s="58" t="s">
-        <v>113</v>
-      </c>
+      <c r="U1872" s="65"/>
       <c r="V1872" s="36" t="s">
         <v>1612</v>
       </c>
@@ -75881,7 +75879,7 @@
         <f t="shared" si="98"/>
         <v>2</v>
       </c>
-      <c r="N2088" s="59" t="s">
+      <c r="N2088" s="58" t="s">
         <v>1036</v>
       </c>
       <c r="U2088" s="1" t="s">
@@ -76221,10 +76219,10 @@
         <f t="shared" si="98"/>
         <v>13</v>
       </c>
-      <c r="N2099" s="59" t="s">
+      <c r="N2099" s="58" t="s">
         <v>1050</v>
       </c>
-      <c r="U2099" s="60" t="s">
+      <c r="U2099" s="59" t="s">
         <v>1605</v>
       </c>
       <c r="V2099" s="36" t="s">
@@ -76253,7 +76251,7 @@
         <f t="shared" si="98"/>
         <v>14</v>
       </c>
-      <c r="N2100" s="59" t="s">
+      <c r="N2100" s="58" t="s">
         <v>1051</v>
       </c>
       <c r="V2100" s="36" t="s">
@@ -77638,7 +77636,7 @@
         <f t="shared" si="101"/>
         <v>59</v>
       </c>
-      <c r="N2145" s="59" t="s">
+      <c r="N2145" s="58" t="s">
         <v>1079</v>
       </c>
       <c r="S2145" s="7" t="s">
@@ -77674,7 +77672,7 @@
         <f t="shared" si="101"/>
         <v>60</v>
       </c>
-      <c r="N2146" s="59" t="s">
+      <c r="N2146" s="58" t="s">
         <v>1504</v>
       </c>
       <c r="P2146" s="7" t="s">
@@ -78557,7 +78555,7 @@
       <c r="P2175" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="V2175" s="62" t="s">
+      <c r="V2175" s="61" t="s">
         <v>1614</v>
       </c>
     </row>
@@ -78925,7 +78923,7 @@
         <f t="shared" si="104"/>
         <v>101</v>
       </c>
-      <c r="N2187" s="59" t="s">
+      <c r="N2187" s="58" t="s">
         <v>225</v>
       </c>
       <c r="V2187" s="36" t="s">
@@ -78954,7 +78952,7 @@
         <f t="shared" si="104"/>
         <v>102</v>
       </c>
-      <c r="N2188" s="59" t="s">
+      <c r="N2188" s="58" t="s">
         <v>1101</v>
       </c>
       <c r="U2188" s="7" t="s">
@@ -78992,7 +78990,7 @@
       <c r="P2189" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="V2189" s="61" t="s">
+      <c r="V2189" s="60" t="s">
         <v>1582</v>
       </c>
     </row>
@@ -82652,7 +82650,7 @@
         <f t="shared" si="107"/>
         <v>221</v>
       </c>
-      <c r="N2307" s="59" t="s">
+      <c r="N2307" s="58" t="s">
         <v>230</v>
       </c>
       <c r="O2307" s="6" t="s">
@@ -85245,7 +85243,7 @@
         <f t="shared" si="113"/>
         <v>303</v>
       </c>
-      <c r="N2389" s="59" t="s">
+      <c r="N2389" s="58" t="s">
         <v>1007</v>
       </c>
       <c r="S2389" s="7" t="s">
@@ -85283,7 +85281,7 @@
         <f t="shared" si="113"/>
         <v>304</v>
       </c>
-      <c r="N2390" s="59" t="s">
+      <c r="N2390" s="58" t="s">
         <v>186</v>
       </c>
       <c r="V2390" s="36" t="s">

</xml_diff>

<commit_message>
nmv 24 10 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 3.4 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 3.4 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066477F2-0F29-48D6-A42B-A5C861161354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B293CD9-BEEB-4812-8085-966DCD96A832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8562" uniqueCount="1619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8562" uniqueCount="1620">
   <si>
     <t>PS</t>
   </si>
@@ -4994,12 +4994,27 @@
   <si>
     <t>GRuqtava#t</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">NE + </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>NRE</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5157,6 +5172,13 @@
     </font>
     <font>
       <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -5704,9 +5726,9 @@
   <dimension ref="A1:V2393"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2295" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2319" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N2311" sqref="N2311"/>
+      <selection pane="bottomLeft" activeCell="N2333" sqref="N2333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -83460,8 +83482,8 @@
       <c r="N2332" s="36" t="s">
         <v>1181</v>
       </c>
-      <c r="U2332" s="7" t="s">
-        <v>130</v>
+      <c r="U2332" s="64" t="s">
+        <v>1619</v>
       </c>
       <c r="V2332" s="36" t="s">
         <v>1608</v>

</xml_diff>